<commit_message>
Registration page and Registration page test
</commit_message>
<xml_diff>
--- a/tables/pet-store-data.xlsx
+++ b/tables/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="615">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1560,6 +1560,306 @@
   </si>
   <si>
     <t>Lorelai50</t>
+  </si>
+  <si>
+    <t>Dayton3</t>
+  </si>
+  <si>
+    <t>Oscar6</t>
+  </si>
+  <si>
+    <t>Keshawn9</t>
+  </si>
+  <si>
+    <t>Madden12</t>
+  </si>
+  <si>
+    <t>Matteo15</t>
+  </si>
+  <si>
+    <t>Tiffany18</t>
+  </si>
+  <si>
+    <t>Odin21</t>
+  </si>
+  <si>
+    <t>Dylan24</t>
+  </si>
+  <si>
+    <t>Jaylee27</t>
+  </si>
+  <si>
+    <t>Julie30</t>
+  </si>
+  <si>
+    <t>Khalil33</t>
+  </si>
+  <si>
+    <t>Jerry36</t>
+  </si>
+  <si>
+    <t>Cecelia39</t>
+  </si>
+  <si>
+    <t>Dax42</t>
+  </si>
+  <si>
+    <t>Linda45</t>
+  </si>
+  <si>
+    <t>Yusuf48</t>
+  </si>
+  <si>
+    <t>Jenna51</t>
+  </si>
+  <si>
+    <t>Ruth54</t>
+  </si>
+  <si>
+    <t>Payten57</t>
+  </si>
+  <si>
+    <t>Meredith60</t>
+  </si>
+  <si>
+    <t>Trent63</t>
+  </si>
+  <si>
+    <t>Camila66</t>
+  </si>
+  <si>
+    <t>Kyson69</t>
+  </si>
+  <si>
+    <t>Yadira72</t>
+  </si>
+  <si>
+    <t>Lucille75</t>
+  </si>
+  <si>
+    <t>Sanaa78</t>
+  </si>
+  <si>
+    <t>Aileen81</t>
+  </si>
+  <si>
+    <t>Leonard84</t>
+  </si>
+  <si>
+    <t>April87</t>
+  </si>
+  <si>
+    <t>Paulina90</t>
+  </si>
+  <si>
+    <t>Nehemiah93</t>
+  </si>
+  <si>
+    <t>Heath96</t>
+  </si>
+  <si>
+    <t>Mikaela99</t>
+  </si>
+  <si>
+    <t>Damari102</t>
+  </si>
+  <si>
+    <t>Haylie105</t>
+  </si>
+  <si>
+    <t>Raul108</t>
+  </si>
+  <si>
+    <t>Kailey111</t>
+  </si>
+  <si>
+    <t>Naima114</t>
+  </si>
+  <si>
+    <t>Dakota117</t>
+  </si>
+  <si>
+    <t>Shelby120</t>
+  </si>
+  <si>
+    <t>Carter123</t>
+  </si>
+  <si>
+    <t>Addyson126</t>
+  </si>
+  <si>
+    <t>Mike129</t>
+  </si>
+  <si>
+    <t>Irvin132</t>
+  </si>
+  <si>
+    <t>Rocco135</t>
+  </si>
+  <si>
+    <t>Julia138</t>
+  </si>
+  <si>
+    <t>Karley141</t>
+  </si>
+  <si>
+    <t>Dustin144</t>
+  </si>
+  <si>
+    <t>Melanie147</t>
+  </si>
+  <si>
+    <t>Lorelai150</t>
+  </si>
+  <si>
+    <t>Dayton2</t>
+  </si>
+  <si>
+    <t>Oscar4</t>
+  </si>
+  <si>
+    <t>Keshawn6</t>
+  </si>
+  <si>
+    <t>Madden8</t>
+  </si>
+  <si>
+    <t>Matteo10</t>
+  </si>
+  <si>
+    <t>Tiffany12</t>
+  </si>
+  <si>
+    <t>Odin14</t>
+  </si>
+  <si>
+    <t>Dylan16</t>
+  </si>
+  <si>
+    <t>Jaylee18</t>
+  </si>
+  <si>
+    <t>Julie20</t>
+  </si>
+  <si>
+    <t>Khalil22</t>
+  </si>
+  <si>
+    <t>Jerry24</t>
+  </si>
+  <si>
+    <t>Cecelia26</t>
+  </si>
+  <si>
+    <t>Dax28</t>
+  </si>
+  <si>
+    <t>Linda30</t>
+  </si>
+  <si>
+    <t>Yusuf32</t>
+  </si>
+  <si>
+    <t>Jenna34</t>
+  </si>
+  <si>
+    <t>Ruth36</t>
+  </si>
+  <si>
+    <t>Payten38</t>
+  </si>
+  <si>
+    <t>Meredith40</t>
+  </si>
+  <si>
+    <t>Trent42</t>
+  </si>
+  <si>
+    <t>Camila44</t>
+  </si>
+  <si>
+    <t>Kyson46</t>
+  </si>
+  <si>
+    <t>Yadira48</t>
+  </si>
+  <si>
+    <t>Lucille50</t>
+  </si>
+  <si>
+    <t>Sanaa52</t>
+  </si>
+  <si>
+    <t>Aileen54</t>
+  </si>
+  <si>
+    <t>Leonard56</t>
+  </si>
+  <si>
+    <t>April58</t>
+  </si>
+  <si>
+    <t>Paulina60</t>
+  </si>
+  <si>
+    <t>Nehemiah62</t>
+  </si>
+  <si>
+    <t>Heath64</t>
+  </si>
+  <si>
+    <t>Mikaela66</t>
+  </si>
+  <si>
+    <t>Damari68</t>
+  </si>
+  <si>
+    <t>Haylie70</t>
+  </si>
+  <si>
+    <t>Raul72</t>
+  </si>
+  <si>
+    <t>Kailey74</t>
+  </si>
+  <si>
+    <t>Naima76</t>
+  </si>
+  <si>
+    <t>Dakota78</t>
+  </si>
+  <si>
+    <t>Shelby80</t>
+  </si>
+  <si>
+    <t>Carter82</t>
+  </si>
+  <si>
+    <t>Addyson84</t>
+  </si>
+  <si>
+    <t>Mike86</t>
+  </si>
+  <si>
+    <t>Irvin88</t>
+  </si>
+  <si>
+    <t>Rocco90</t>
+  </si>
+  <si>
+    <t>Julia92</t>
+  </si>
+  <si>
+    <t>Karley94</t>
+  </si>
+  <si>
+    <t>Dustin96</t>
+  </si>
+  <si>
+    <t>Melanie98</t>
+  </si>
+  <si>
+    <t>Lorelai100</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2496,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>465</v>
+        <v>565</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2234,7 +2534,7 @@
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>466</v>
+        <v>566</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2272,7 +2572,7 @@
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>467</v>
+        <v>567</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2310,7 +2610,7 @@
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>468</v>
+        <v>568</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2348,7 +2648,7 @@
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>469</v>
+        <v>569</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2386,7 +2686,7 @@
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>470</v>
+        <v>570</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2424,7 +2724,7 @@
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>471</v>
+        <v>571</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2462,7 +2762,7 @@
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>472</v>
+        <v>572</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2500,7 +2800,7 @@
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>473</v>
+        <v>573</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2538,7 +2838,7 @@
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>474</v>
+        <v>574</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2576,7 +2876,7 @@
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>475</v>
+        <v>575</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2614,7 +2914,7 @@
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>476</v>
+        <v>576</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -2652,7 +2952,7 @@
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>477</v>
+        <v>577</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2690,7 +2990,7 @@
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>478</v>
+        <v>578</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -2728,7 +3028,7 @@
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>479</v>
+        <v>579</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -2766,7 +3066,7 @@
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>480</v>
+        <v>580</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -2804,7 +3104,7 @@
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>481</v>
+        <v>581</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -2842,7 +3142,7 @@
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>482</v>
+        <v>582</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -2880,7 +3180,7 @@
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>483</v>
+        <v>583</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -2918,7 +3218,7 @@
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>484</v>
+        <v>584</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -2956,7 +3256,7 @@
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>485</v>
+        <v>585</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -2994,7 +3294,7 @@
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>486</v>
+        <v>586</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3032,7 +3332,7 @@
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>487</v>
+        <v>587</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3070,7 +3370,7 @@
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>488</v>
+        <v>588</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3108,7 +3408,7 @@
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>489</v>
+        <v>589</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3146,7 +3446,7 @@
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>490</v>
+        <v>590</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3184,7 +3484,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>491</v>
+        <v>591</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3222,7 +3522,7 @@
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>492</v>
+        <v>592</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3260,7 +3560,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>493</v>
+        <v>593</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3298,7 +3598,7 @@
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>494</v>
+        <v>594</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3336,7 +3636,7 @@
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>495</v>
+        <v>595</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3374,7 +3674,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>496</v>
+        <v>596</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3412,7 +3712,7 @@
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>497</v>
+        <v>597</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3450,7 +3750,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>498</v>
+        <v>598</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3488,7 +3788,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>499</v>
+        <v>599</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3526,7 +3826,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -3564,7 +3864,7 @@
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>501</v>
+        <v>601</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -3602,7 +3902,7 @@
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>502</v>
+        <v>602</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -3640,7 +3940,7 @@
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>503</v>
+        <v>603</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -3678,7 +3978,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>504</v>
+        <v>604</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -3716,7 +4016,7 @@
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>505</v>
+        <v>605</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -3754,7 +4054,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>506</v>
+        <v>606</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -3792,7 +4092,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>507</v>
+        <v>607</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -3830,7 +4130,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>508</v>
+        <v>608</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -3868,7 +4168,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>509</v>
+        <v>609</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -3906,7 +4206,7 @@
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>510</v>
+        <v>610</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -3944,7 +4244,7 @@
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>511</v>
+        <v>611</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -3982,7 +4282,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>512</v>
+        <v>612</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4020,7 +4320,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>513</v>
+        <v>613</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4058,7 +4358,7 @@
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>514</v>
+        <v>614</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>

</xml_diff>